<commit_message>
AAL added to AFS
</commit_message>
<xml_diff>
--- a/specifications/afs/Business intelligence systems - System Development - BI Project - Finance Systems - AFS Data Specification V4.35.xlsx
+++ b/specifications/afs/Business intelligence systems - System Development - BI Project - Finance Systems - AFS Data Specification V4.35.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ShrForms\specifications\afs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59BB02F-3892-43EE-9CF7-80C5DA76EA17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FCA17D-8CE0-4AE5-B1B6-604C4FBE6DB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14105,11 +14105,11 @@
   <dimension ref="A1:AG627"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B619" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B605" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="B6" sqref="B6"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H619" sqref="H619"/>
+      <selection pane="bottomRight" activeCell="I119" sqref="I119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -19910,9 +19910,9 @@
         <v>225</v>
       </c>
       <c r="H119" s="38"/>
-      <c r="I119" s="269">
-        <f>SUM(H117,H118)</f>
-        <v>162807</v>
+      <c r="I119" s="269" t="str">
+        <f>A608</f>
+        <v>AFSF002</v>
       </c>
       <c r="J119" s="37"/>
       <c r="K119" s="146"/>
@@ -20122,7 +20122,7 @@
       <c r="H123" s="38"/>
       <c r="I123" s="214">
         <f>SUM(H116,I119,H120,H121,H122)</f>
-        <v>168822</v>
+        <v>6015</v>
       </c>
       <c r="J123" s="37"/>
       <c r="K123" s="146"/>
@@ -20838,7 +20838,7 @@
       <c r="H137" s="38"/>
       <c r="I137" s="214">
         <f>SUM(I123,H124,I136)</f>
-        <v>168931</v>
+        <v>6124</v>
       </c>
       <c r="J137" s="37"/>
       <c r="K137" s="146"/>
@@ -21292,7 +21292,7 @@
       <c r="H146" s="38"/>
       <c r="I146" s="214">
         <f>SUM(I137,I145)</f>
-        <v>44418</v>
+        <v>-118389</v>
       </c>
       <c r="J146" s="37"/>
       <c r="K146" s="146"/>
@@ -21612,7 +21612,7 @@
       <c r="M152" s="146"/>
       <c r="N152" s="37" t="b">
         <f>I152=I146</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O152" s="146" t="s">
         <v>249</v>
@@ -45057,8 +45057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:XFC31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -45442,8 +45442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -45941,7 +45941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:XFB64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -46041,9 +46041,9 @@
       <c r="A9" s="231" t="s">
         <v>157</v>
       </c>
-      <c r="B9" s="232">
+      <c r="B9" s="232" t="str">
         <f>Data!I119</f>
-        <v>162807</v>
+        <v>AFSF002</v>
       </c>
       <c r="C9" s="121"/>
       <c r="D9" s="100"/>
@@ -46115,7 +46115,7 @@
       </c>
       <c r="B15" s="232">
         <f>Data!I123</f>
-        <v>168822</v>
+        <v>6015</v>
       </c>
       <c r="C15" s="121"/>
       <c r="D15" s="100"/>
@@ -46359,7 +46359,7 @@
       </c>
       <c r="B37" s="232">
         <f>Data!I137</f>
-        <v>168931</v>
+        <v>6124</v>
       </c>
       <c r="C37" s="121"/>
       <c r="D37" s="100"/>
@@ -46515,7 +46515,7 @@
       </c>
       <c r="B51" s="232">
         <f>Data!I146</f>
-        <v>44418</v>
+        <v>-118389</v>
       </c>
       <c r="C51" s="121"/>
       <c r="D51" s="100"/>
@@ -46658,7 +46658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:XFB33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>

</xml_diff>